<commit_message>
correct tiny errors and rephrase some comments.
</commit_message>
<xml_diff>
--- a/NetworkConfigData/NETS_NYPS_68bus_detuned_gov_FS.xlsx
+++ b/NetworkConfigData/NETS_NYPS_68bus_detuned_gov_FS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Greybox_Case_Study\Examples\Paper_GreyBox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Simplex-Power-Systems\NetworkConfigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EFB16B-CEE7-4EDA-897D-9E111938A877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68ED9A3C-3AD9-477C-BC3D-A0DDA7946D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -3440,8 +3440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:AQ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5343,7 +5343,7 @@
         <v>0.03</v>
       </c>
       <c r="G22" s="9">
-        <v>3.0000000000000001E-3</v>
+        <v>9.55E-6</v>
       </c>
       <c r="H22" s="9">
         <v>0</v>

</xml_diff>